<commit_message>
Added ability to go from SMILES to Mol and real data set
</commit_message>
<xml_diff>
--- a/toy_data.xlsx
+++ b/toy_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\pythonScripts\MSlibrary-generation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\pythonScripts\Mtb_inhibition\Mtb_inhibition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFE27FC6-00A3-4516-8EE6-6164FB391B77}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C9B7A97-21D5-40EC-96B0-BA14F8D80A04}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5076" xr2:uid="{F52E7153-7355-4B45-8E7B-A0D46EAB1AA7}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="219">
   <si>
     <t>id</t>
   </si>
@@ -54,27 +54,6 @@
     <t>ms id</t>
   </si>
   <si>
-    <t>cpd02920_c0</t>
-  </si>
-  <si>
-    <t>2-Amino-4-hydroxy-6-hydroxymethyl-7-8-dihydropteridinediphosphate_c0</t>
-  </si>
-  <si>
-    <t>C7H9N5O8P2</t>
-  </si>
-  <si>
-    <t>FCQGJGLSOWZZON-UHFFFAOYSA-L</t>
-  </si>
-  <si>
-    <t>N=c1nc([O-])c2c([nH]1)NCC(COP(=O)(O)OP(=O)([O-])O)=N2</t>
-  </si>
-  <si>
-    <t>C04807</t>
-  </si>
-  <si>
-    <t>cpd02920</t>
-  </si>
-  <si>
     <t>cpd00683_c0</t>
   </si>
   <si>
@@ -306,27 +285,6 @@
     <t>cpd00046</t>
   </si>
   <si>
-    <t>cpd00096_c0</t>
-  </si>
-  <si>
-    <t>CDP_c0</t>
-  </si>
-  <si>
-    <t>C9H13N3O11P2</t>
-  </si>
-  <si>
-    <t>ZWIADYZPOWUWEW-XVFCMESISA-L</t>
-  </si>
-  <si>
-    <t>N=c1ccn(C2OC(COP(=O)(O)OP(=O)([O-])O)C(O)C2O)c([O-])n1</t>
-  </si>
-  <si>
-    <t>C00112</t>
-  </si>
-  <si>
-    <t>cpd00096</t>
-  </si>
-  <si>
     <t>cpd00037_c0</t>
   </si>
   <si>
@@ -621,27 +579,6 @@
     <t>cpd00982</t>
   </si>
   <si>
-    <t>cpd00533_c0</t>
-  </si>
-  <si>
-    <t>dCDP_c0</t>
-  </si>
-  <si>
-    <t>C9H13N3O10P2</t>
-  </si>
-  <si>
-    <t>FTDHDKPUHBLBTL-SHYZEUOFSA-L</t>
-  </si>
-  <si>
-    <t>N=c1ccn(C2CC(O)C(COP(=O)(O)OP(=O)([O-])O)O2)c([O-])n1</t>
-  </si>
-  <si>
-    <t>C00705</t>
-  </si>
-  <si>
-    <t>cpd00533</t>
-  </si>
-  <si>
     <t>cpd00356_c0</t>
   </si>
   <si>
@@ -684,27 +621,6 @@
     <t>cpd00213</t>
   </si>
   <si>
-    <t>cpd03049_c0</t>
-  </si>
-  <si>
-    <t>2-Hydroxyethyl-ThPP_c0</t>
-  </si>
-  <si>
-    <t>C14H21N4O8P2S</t>
-  </si>
-  <si>
-    <t>RRUVJGASJONMDY-UHFFFAOYSA-M</t>
-  </si>
-  <si>
-    <t>Cc1ncc(C[n+]2c(C(C)O)sc(CCOP(=O)([O-])OP(=O)([O-])O)c2C)c(=N)[nH]1</t>
-  </si>
-  <si>
-    <t>C05125</t>
-  </si>
-  <si>
-    <t>cpd03049</t>
-  </si>
-  <si>
     <t>cpd00056_c0</t>
   </si>
   <si>
@@ -766,27 +682,6 @@
   </si>
   <si>
     <t>cpd00006</t>
-  </si>
-  <si>
-    <t>cpd00842_c0</t>
-  </si>
-  <si>
-    <t>(S)-3-Hydroxybutyryl-CoA_c0</t>
-  </si>
-  <si>
-    <t>C25H38N7O18P3S</t>
-  </si>
-  <si>
-    <t>QHHKKMYHDBRONY-BEVJUKKNSA-J</t>
-  </si>
-  <si>
-    <t>CC(O)CC(=O)SCCN=C([O-])CCN=C([O-])C(O)C(C)(C)COP(=O)(O)OP(=O)(O)OCC1OC(n2cnc3c(N)ncnc32)C(O)C1OP(=O)([O-])[O-]</t>
-  </si>
-  <si>
-    <t>C01144</t>
-  </si>
-  <si>
-    <t>cpd00842</t>
   </si>
 </sst>
 </file>
@@ -1138,13 +1033,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E16355B-364D-4D3C-B1EF-7FB5DD73F55C}">
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:XFD25"/>
+    <sheetView tabSelected="1" topLeftCell="B5" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="41.44140625" customWidth="1"/>
+    <col min="5" max="5" width="45.109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -1186,7 +1085,7 @@
         <v>11</v>
       </c>
       <c r="D2">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="E2" t="s">
         <v>12</v>
@@ -1195,7 +1094,7 @@
         <v>13</v>
       </c>
       <c r="G2">
-        <v>-423.61</v>
+        <v>12.16</v>
       </c>
       <c r="H2" t="s">
         <v>14</v>
@@ -1204,7 +1103,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -1215,7 +1114,7 @@
         <v>18</v>
       </c>
       <c r="D3">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="E3" t="s">
         <v>19</v>
@@ -1224,7 +1123,7 @@
         <v>20</v>
       </c>
       <c r="G3">
-        <v>12.16</v>
+        <v>-66.63</v>
       </c>
       <c r="H3" t="s">
         <v>21</v>
@@ -1244,7 +1143,7 @@
         <v>25</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="E4" t="s">
         <v>26</v>
@@ -1253,7 +1152,7 @@
         <v>27</v>
       </c>
       <c r="G4">
-        <v>-66.63</v>
+        <v>-115.31</v>
       </c>
       <c r="H4" t="s">
         <v>28</v>
@@ -1262,7 +1161,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -1273,7 +1172,7 @@
         <v>32</v>
       </c>
       <c r="D5">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="E5" t="s">
         <v>33</v>
@@ -1282,7 +1181,7 @@
         <v>34</v>
       </c>
       <c r="G5">
-        <v>-115.31</v>
+        <v>-75.91</v>
       </c>
       <c r="H5" t="s">
         <v>35</v>
@@ -1302,7 +1201,7 @@
         <v>39</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E6" t="s">
         <v>40</v>
@@ -1311,7 +1210,7 @@
         <v>41</v>
       </c>
       <c r="G6">
-        <v>-75.91</v>
+        <v>-109.02</v>
       </c>
       <c r="H6" t="s">
         <v>42</v>
@@ -1331,7 +1230,7 @@
         <v>46</v>
       </c>
       <c r="D7">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="E7" t="s">
         <v>47</v>
@@ -1340,7 +1239,7 @@
         <v>48</v>
       </c>
       <c r="G7">
-        <v>-109.02</v>
+        <v>-9.1199999999999992</v>
       </c>
       <c r="H7" t="s">
         <v>49</v>
@@ -1360,7 +1259,7 @@
         <v>53</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="E8" t="s">
         <v>54</v>
@@ -1369,7 +1268,7 @@
         <v>55</v>
       </c>
       <c r="G8">
-        <v>-9.1199999999999992</v>
+        <v>-785.83</v>
       </c>
       <c r="H8" t="s">
         <v>56</v>
@@ -1389,7 +1288,7 @@
         <v>60</v>
       </c>
       <c r="D9">
-        <v>-4</v>
+        <v>0</v>
       </c>
       <c r="E9" t="s">
         <v>61</v>
@@ -1398,7 +1297,7 @@
         <v>62</v>
       </c>
       <c r="G9">
-        <v>-785.83</v>
+        <v>-124.15</v>
       </c>
       <c r="H9" t="s">
         <v>63</v>
@@ -1418,7 +1317,7 @@
         <v>67</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="E10" t="s">
         <v>68</v>
@@ -1427,7 +1326,7 @@
         <v>69</v>
       </c>
       <c r="G10">
-        <v>-124.15</v>
+        <v>-751.99400000000003</v>
       </c>
       <c r="H10" t="s">
         <v>70</v>
@@ -1447,7 +1346,7 @@
         <v>74</v>
       </c>
       <c r="D11">
-        <v>-4</v>
+        <v>0</v>
       </c>
       <c r="E11" t="s">
         <v>75</v>
@@ -1456,7 +1355,7 @@
         <v>76</v>
       </c>
       <c r="G11">
-        <v>-751.99400000000003</v>
+        <v>-161.6</v>
       </c>
       <c r="H11" t="s">
         <v>77</v>
@@ -1476,7 +1375,7 @@
         <v>81</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="E12" t="s">
         <v>82</v>
@@ -1485,7 +1384,7 @@
         <v>83</v>
       </c>
       <c r="G12">
-        <v>-161.6</v>
+        <v>-345.38</v>
       </c>
       <c r="H12" t="s">
         <v>84</v>
@@ -1514,7 +1413,7 @@
         <v>90</v>
       </c>
       <c r="G13">
-        <v>-345.38</v>
+        <v>-756.9</v>
       </c>
       <c r="H13" t="s">
         <v>91</v>
@@ -1534,7 +1433,7 @@
         <v>95</v>
       </c>
       <c r="D14">
-        <v>-2</v>
+        <v>-4</v>
       </c>
       <c r="E14" t="s">
         <v>96</v>
@@ -1543,7 +1442,7 @@
         <v>97</v>
       </c>
       <c r="G14">
-        <v>-553.38</v>
+        <v>-678.6</v>
       </c>
       <c r="H14" t="s">
         <v>98</v>
@@ -1572,7 +1471,7 @@
         <v>104</v>
       </c>
       <c r="G15">
-        <v>-756.9</v>
+        <v>-605.77</v>
       </c>
       <c r="H15" t="s">
         <v>105</v>
@@ -1601,7 +1500,7 @@
         <v>111</v>
       </c>
       <c r="G16">
-        <v>-678.6</v>
+        <v>-831.43</v>
       </c>
       <c r="H16" t="s">
         <v>112</v>
@@ -1630,7 +1529,7 @@
         <v>118</v>
       </c>
       <c r="G17">
-        <v>-605.77</v>
+        <v>-257.85000000000002</v>
       </c>
       <c r="H17" t="s">
         <v>119</v>
@@ -1650,7 +1549,7 @@
         <v>123</v>
       </c>
       <c r="D18">
-        <v>-4</v>
+        <v>-1</v>
       </c>
       <c r="E18" t="s">
         <v>124</v>
@@ -1659,7 +1558,7 @@
         <v>125</v>
       </c>
       <c r="G18">
-        <v>-831.43</v>
+        <v>-164.13</v>
       </c>
       <c r="H18" t="s">
         <v>126</v>
@@ -1679,7 +1578,7 @@
         <v>130</v>
       </c>
       <c r="D19">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="E19" t="s">
         <v>131</v>
@@ -1688,7 +1587,7 @@
         <v>132</v>
       </c>
       <c r="G19">
-        <v>-257.85000000000002</v>
+        <v>-83.394000000000005</v>
       </c>
       <c r="H19" t="s">
         <v>133</v>
@@ -1717,7 +1616,7 @@
         <v>139</v>
       </c>
       <c r="G20">
-        <v>-164.13</v>
+        <v>-190.374</v>
       </c>
       <c r="H20" t="s">
         <v>140</v>
@@ -1737,7 +1636,7 @@
         <v>144</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="E21" t="s">
         <v>145</v>
@@ -1746,7 +1645,7 @@
         <v>146</v>
       </c>
       <c r="G21">
-        <v>-83.394000000000005</v>
+        <v>-164.58</v>
       </c>
       <c r="H21" t="s">
         <v>147</v>
@@ -1775,7 +1674,7 @@
         <v>153</v>
       </c>
       <c r="G22">
-        <v>-190.374</v>
+        <v>-88.29</v>
       </c>
       <c r="H22" t="s">
         <v>154</v>
@@ -1795,7 +1694,7 @@
         <v>158</v>
       </c>
       <c r="D23">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="E23" t="s">
         <v>159</v>
@@ -1804,7 +1703,7 @@
         <v>160</v>
       </c>
       <c r="G23">
-        <v>-164.58</v>
+        <v>-515.07000000000005</v>
       </c>
       <c r="H23" t="s">
         <v>161</v>
@@ -1824,7 +1723,7 @@
         <v>165</v>
       </c>
       <c r="D24">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="E24" t="s">
         <v>166</v>
@@ -1833,7 +1732,7 @@
         <v>167</v>
       </c>
       <c r="G24">
-        <v>-88.29</v>
+        <v>-201</v>
       </c>
       <c r="H24" t="s">
         <v>168</v>
@@ -1853,7 +1752,7 @@
         <v>172</v>
       </c>
       <c r="D25">
-        <v>-3</v>
+        <v>-2</v>
       </c>
       <c r="E25" t="s">
         <v>173</v>
@@ -1862,7 +1761,7 @@
         <v>174</v>
       </c>
       <c r="G25">
-        <v>-515.07000000000005</v>
+        <v>-190.52</v>
       </c>
       <c r="H25" t="s">
         <v>175</v>
@@ -1891,7 +1790,7 @@
         <v>181</v>
       </c>
       <c r="G26">
-        <v>-201</v>
+        <v>-538.17999999999995</v>
       </c>
       <c r="H26" t="s">
         <v>182</v>
@@ -1911,7 +1810,7 @@
         <v>186</v>
       </c>
       <c r="D27">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="E27" t="s">
         <v>187</v>
@@ -1920,7 +1819,7 @@
         <v>188</v>
       </c>
       <c r="G27">
-        <v>-190.52</v>
+        <v>-721.54</v>
       </c>
       <c r="H27" t="s">
         <v>189</v>
@@ -1940,7 +1839,7 @@
         <v>193</v>
       </c>
       <c r="D28">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="E28" t="s">
         <v>194</v>
@@ -1949,7 +1848,7 @@
         <v>195</v>
       </c>
       <c r="G28">
-        <v>-538.17999999999995</v>
+        <v>-21.54</v>
       </c>
       <c r="H28" t="s">
         <v>196</v>
@@ -1969,7 +1868,7 @@
         <v>200</v>
       </c>
       <c r="D29">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="E29" t="s">
         <v>201</v>
@@ -1978,7 +1877,7 @@
         <v>202</v>
       </c>
       <c r="G29">
-        <v>-513.54</v>
+        <v>-368.32</v>
       </c>
       <c r="H29" t="s">
         <v>203</v>
@@ -1998,7 +1897,7 @@
         <v>207</v>
       </c>
       <c r="D30">
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="E30" t="s">
         <v>208</v>
@@ -2007,7 +1906,7 @@
         <v>209</v>
       </c>
       <c r="G30">
-        <v>-721.54</v>
+        <v>-61.183999999999997</v>
       </c>
       <c r="H30" t="s">
         <v>210</v>
@@ -2027,7 +1926,7 @@
         <v>214</v>
       </c>
       <c r="D31">
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="E31" t="s">
         <v>215</v>
@@ -2036,158 +1935,13 @@
         <v>216</v>
       </c>
       <c r="G31">
-        <v>-21.54</v>
+        <v>-742.09</v>
       </c>
       <c r="H31" t="s">
         <v>217</v>
       </c>
       <c r="I31" t="s">
         <v>218</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>219</v>
-      </c>
-      <c r="B32" t="s">
-        <v>220</v>
-      </c>
-      <c r="C32" t="s">
-        <v>221</v>
-      </c>
-      <c r="D32">
-        <v>-1</v>
-      </c>
-      <c r="E32" t="s">
-        <v>222</v>
-      </c>
-      <c r="F32" t="s">
-        <v>223</v>
-      </c>
-      <c r="G32">
-        <v>-405.15</v>
-      </c>
-      <c r="H32" t="s">
-        <v>224</v>
-      </c>
-      <c r="I32" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>226</v>
-      </c>
-      <c r="B33" t="s">
-        <v>227</v>
-      </c>
-      <c r="C33" t="s">
-        <v>228</v>
-      </c>
-      <c r="D33">
-        <v>-1</v>
-      </c>
-      <c r="E33" t="s">
-        <v>229</v>
-      </c>
-      <c r="F33" t="s">
-        <v>230</v>
-      </c>
-      <c r="G33">
-        <v>-368.32</v>
-      </c>
-      <c r="H33" t="s">
-        <v>231</v>
-      </c>
-      <c r="I33" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>233</v>
-      </c>
-      <c r="B34" t="s">
-        <v>234</v>
-      </c>
-      <c r="C34" t="s">
-        <v>235</v>
-      </c>
-      <c r="D34">
-        <v>0</v>
-      </c>
-      <c r="E34" t="s">
-        <v>236</v>
-      </c>
-      <c r="F34" t="s">
-        <v>237</v>
-      </c>
-      <c r="G34">
-        <v>-61.183999999999997</v>
-      </c>
-      <c r="H34" t="s">
-        <v>238</v>
-      </c>
-      <c r="I34" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>240</v>
-      </c>
-      <c r="B35" t="s">
-        <v>241</v>
-      </c>
-      <c r="C35" t="s">
-        <v>242</v>
-      </c>
-      <c r="D35">
-        <v>-3</v>
-      </c>
-      <c r="E35" t="s">
-        <v>243</v>
-      </c>
-      <c r="F35" t="s">
-        <v>244</v>
-      </c>
-      <c r="G35">
-        <v>-742.09</v>
-      </c>
-      <c r="H35" t="s">
-        <v>245</v>
-      </c>
-      <c r="I35" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>247</v>
-      </c>
-      <c r="B36" t="s">
-        <v>248</v>
-      </c>
-      <c r="C36" t="s">
-        <v>249</v>
-      </c>
-      <c r="D36">
-        <v>-4</v>
-      </c>
-      <c r="E36" t="s">
-        <v>250</v>
-      </c>
-      <c r="F36" t="s">
-        <v>251</v>
-      </c>
-      <c r="G36">
-        <v>-820.63</v>
-      </c>
-      <c r="H36" t="s">
-        <v>252</v>
-      </c>
-      <c r="I36" t="s">
-        <v>253</v>
       </c>
     </row>
   </sheetData>

</xml_diff>